<commit_message>
tried to add sec y axis to facet grid without success
</commit_message>
<xml_diff>
--- a/data/ICES_stock_cat.xlsx
+++ b/data/ICES_stock_cat.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -370,6 +370,16 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Name_FR</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Name_EN</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Stock category</t>
         </is>
       </c>
@@ -387,6 +397,16 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Ange de mer commun</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Angelshark</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -404,6 +424,16 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Requin-pèlerin</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Basking shark</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -419,7 +449,7 @@
           <t>Centrophorus squamosus, Centroscymnus coelolepis</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -438,6 +468,16 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>Aiguillat commun</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Picked dogfish</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
@@ -455,6 +495,16 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>Requin hâ</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Tope shark</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
@@ -472,6 +522,16 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>Squale-chagrin de l'Atlantique</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Leafscale gulper shark</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -489,6 +549,16 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Requin-taupe commun</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Porbeagle</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -504,7 +574,7 @@
           <t>Rajidae</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -521,7 +591,7 @@
           <t>Rajidae</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -538,7 +608,7 @@
           <t>Rajidae</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -555,7 +625,7 @@
           <t>Rajidae</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -574,6 +644,16 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>Raie blanche</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>White skate</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -591,6 +671,16 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>Pocheteau gris</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Blue skate</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -608,6 +698,16 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>Pocheteau gris</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Blue skate</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -625,6 +725,16 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>Pocheteau gris</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Blue skate</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -642,6 +752,16 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>Raie bouclée</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Thornback ray</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -659,6 +779,16 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>Raie bouclée</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Thornback ray</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -676,6 +806,16 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>Raie bouclée</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Thornback ray</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -693,6 +833,16 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>Raie bouclée</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Thornback ray</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
@@ -710,6 +860,16 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>Raie bouclée</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Thornback ray</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -727,6 +887,16 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>Raie bouclée</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Thornback ray</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -744,6 +914,16 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>Raie mêlée</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Small-eyed ray</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
@@ -761,6 +941,16 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>Raie mêlée</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Small-eyed ray</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -778,6 +968,16 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>Raie chardon</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Shagreen ray</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
@@ -795,6 +995,16 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>Raie lisse</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Blonde ray</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
@@ -812,6 +1022,16 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>Raie lisse</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Blonde ray</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -829,6 +1049,16 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>Raie lisse</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Blonde ray</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
@@ -846,6 +1076,16 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>Raie lisse</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Blonde ray</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
@@ -863,6 +1103,16 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>Raie lisse</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Blonde ray</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -880,6 +1130,16 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
+          <t>Raie circulaire</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Sandy ray</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
@@ -897,6 +1157,16 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
+          <t>Raie douce</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Spotted ray</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -914,6 +1184,16 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
+          <t>Raie douce</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Spotted ray</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -931,6 +1211,16 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t>Raie douce</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Spotted ray</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -948,6 +1238,16 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
+          <t>Raie douce</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Spotted ray</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -965,6 +1265,16 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>Raie douce</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Spotted ray</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -982,6 +1292,16 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
+          <t>Raie fleurie</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Cuckoo ray</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -999,6 +1319,16 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
+          <t>Raie fleurie</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Cuckoo ray</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -1016,6 +1346,16 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
+          <t>Raie fleurie</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Cuckoo ray</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -1033,6 +1373,16 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
+          <t>Raie fleurie</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Cuckoo ray</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -1050,6 +1400,16 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
+          <t>Raie radiée épineuse</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Starry ray</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -1067,6 +1427,16 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
+          <t>Raie brunette</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Undulate ray</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -1084,6 +1454,16 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
+          <t>Raie brunette</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Undulate ray</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -1101,6 +1481,16 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
+          <t>Raie brunette</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Undulate ray</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -1118,6 +1508,16 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
+          <t>Raie brunette</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Undulate ray</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -1135,6 +1535,16 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
+          <t>Raie brunette</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Undulate ray</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -1152,6 +1562,16 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
+          <t>Squale-liche</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Kitefin shark</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
@@ -1169,6 +1589,16 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
+          <t>Émissole tachetée</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Starry smooth-hound</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -1186,6 +1616,16 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
+          <t>Chien espagnol</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Blackmouth catshark</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -1203,6 +1643,16 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
+          <t>Chien espagnol</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Blackmouth catshark</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -1220,6 +1670,16 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
+          <t>Petite roussette</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Lesser spotted dogfish</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -1237,6 +1697,16 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
+          <t>Petite roussette</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Lesser spotted dogfish</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -1254,6 +1724,16 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
+          <t>Petite roussette</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Lesser spotted dogfish</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -1271,6 +1751,16 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
+          <t>Petite roussette</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Lesser spotted dogfish</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -1288,6 +1778,16 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
+          <t>Grande roussette</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Nursehound</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
@@ -1303,7 +1803,7 @@
           <t>Alopias</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>6</t>
         </is>

</xml_diff>